<commit_message>
Controle de Caixa Outubro
</commit_message>
<xml_diff>
--- a/CONTROLE DE CAIXA OUTUBRO 2019/04-10-2019_FluxoDeCaixa.xlsx
+++ b/CONTROLE DE CAIXA OUTUBRO 2019/04-10-2019_FluxoDeCaixa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael_Campos\Documents\GitHub\ConnectFibra\CONTROLE DE CAIXA OUTUBRO 2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF36996-F840-495C-B8D0-7B59141E2FEE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA53AE23-532E-494A-9A18-A0B447557994}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9152A456-9720-4D0C-842A-50118CAD28D0}"/>
   </bookViews>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF5ADB1-AEA5-4558-B31C-D3F166D0CCA5}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +546,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="5">
-        <v>43741</v>
+        <v>43742</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>